<commit_message>
Add changes to Leadership prinicples..
</commit_message>
<xml_diff>
--- a/Prep/Amazon/LeaderShipPrinciples.xlsx
+++ b/Prep/Amazon/LeaderShipPrinciples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Items\DSA\Algorithms\Prep\Amazon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D6AC6E5-B6D1-423D-BF9B-0DAFFFD54536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BE0B59-6E77-4005-B6AA-3831D363C190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F254A1FC-440D-4643-80B3-1DB40E3DAEFC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F254A1FC-440D-4643-80B3-1DB40E3DAEFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Obsession" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
   <si>
     <t>Have Back Bone; Disagreement &amp; Commitment</t>
   </si>
@@ -188,6 +188,50 @@
   </si>
   <si>
     <t>Leaders focus on the key inputs for their business and deliver them with the right quality and in a timely fashion. Despite setbacks, they rise to the occasion and never settle.</t>
+  </si>
+  <si>
+    <t>Microsoft was using Tenant Data store for Office 365 Admin Center Webapi's.
+My Team Lead picked up that work item and it was time sensitive task and
+Microsoft was retiring Tenant Data store in next two months. After a month my TeamLead
+had to leave the project as he got another Full time project. I have taken this task 
+to get it complete in a month based upon intial analysis made by my Team Lead.
+Based upon intial analysis I came know that I have to migrate from Tenant Data store to
+Azure Cosmos DB. Make API code changes to use Azure Cosmos DB and Remove Tenant Data store.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I created some of the below steps:
+step1: Create a POC to get connect to azure cosmos db collection and perform
+       Update, Read/Write and Delete operations.
+step2: Migrate existing data from TDS to AZCDB
+step3: Make API changes to use Azure Cosmos DB instead of Tenant Data store.
+step4: Apply POC implementation on API.
+step5: Update unit tests and integration tests.
+Step 6: Demo and Get approval.
+step 7: Deploy it Production and make it available for 10% users using A/B test methods.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action:
+1. At that time I was new to perform CRUD operations on Azure Cosmos DB.
+   I created a POC to perform READ/Write opearation on Azure Cosmos DB test collection.
+   I used Azure SDK to get connect to Azure Cosmos DB collection and Used Azure Libraries to
+   Insert, Update, Delete to Azure Cosmos DB collection.
+   I demoed it to the Team and Team accepted my POC. 
+2. Migrate the data from Tenant Data store(Key Value pair data) to Azure Cosmos DB.
+3. Web api's using Tenant data store to  read/write/update/delete the data. Made
+   api code changes to read/write from Tenant data store to Azure Cosmos DB.
+4. Based upon POC, I applied that implementation to actual API's.
+5. Deployed the code to Test environments to give a demo Tenant Data Store vs Azure Cosmos DB.
+5. Gave a demo of my code changes and team was happy with my code changes.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result:
+The Api ran successfully as it ran on Tenant data store, after migrating to Azure Cosmos DB.
+I deployed the old code to Test01 server and new code to Test02 environments. Compared the results
+on both servers and demo the same to the team. Team was happy with the implementation. Team approved my changes to get it deployed
+to production to get it released to 10% of the website users and monitor for few days. After monitoring,
+No issues were reported and then made it available to 100% users.  </t>
   </si>
 </sst>
 </file>
@@ -622,7 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EC0F6A-74B4-4826-99DF-2CB00802D06B}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -908,17 +952,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C82DE0C8-7F23-4B3F-8DE8-448439008445}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" customWidth="1"/>
-    <col min="3" max="3" width="33.44140625" customWidth="1"/>
+    <col min="1" max="1" width="58" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
     <col min="4" max="4" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -947,6 +991,20 @@
       </c>
       <c r="D3" s="6" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="217.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>